<commit_message>
Added scenario # column
</commit_message>
<xml_diff>
--- a/Excel sheets/Examples/Chapter 6/LookupValue Test Plan breakdown - final stage.xlsx
+++ b/Excel sheets/Examples/Chapter 6/LookupValue Test Plan breakdown - final stage.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f2a63c87061b9b9b/Projects/Books/Automated Testing in Microsoft Dynamics 365 Business Central/2nd Edition/Source/Book/WORD/Chapter 6 - In Progress/Test Plan ^0 Test Design/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lvvugt\source\repos\Automated-Testing-in-Microsoft-Dynamics-365-Business-Central-Second-Edition\Excel sheets\Examples\Chapter 6\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="45" documentId="13_ncr:1_{BAE623AF-B4E1-49DD-847F-1E777F18503D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{CB3B4D2F-9837-4DFC-BD17-DE81E69AC842}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77B5D43C-BDFC-4483-9DD2-11C2A58770FF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-21930" yWindow="1650" windowWidth="18135" windowHeight="13245" xr2:uid="{37BCB399-09BD-4B93-AAF4-793E3BF59A9F}"/>
+    <workbookView xWindow="-22650" yWindow="645" windowWidth="18360" windowHeight="13290" xr2:uid="{37BCB399-09BD-4B93-AAF4-793E3BF59A9F}"/>
   </bookViews>
   <sheets>
     <sheet name="ATDD Scenarios" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="56">
   <si>
     <t>Feature</t>
   </si>
@@ -199,12 +199,18 @@
   </si>
   <si>
     <t>Contact</t>
+  </si>
+  <si>
+    <t>Scenario #</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0000"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -246,7 +252,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -271,11 +277,30 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
+  <dxfs count="9">
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0000"/>
+      <alignment horizontal="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -297,7 +322,24 @@
       </fill>
     </dxf>
     <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -322,15 +364,16 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D26859EB-C8DA-46B9-9E4C-0C2909BE7347}" name="Table29" displayName="Table29" ref="A1:F40" totalsRowShown="0" headerRowDxfId="5">
-  <autoFilter ref="A1:F40" xr:uid="{74C06549-5BDA-49EA-8217-9DE86359CCAF}"/>
-  <tableColumns count="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D26859EB-C8DA-46B9-9E4C-0C2909BE7347}" name="Table29" displayName="Table29" ref="A1:G40" totalsRowShown="0" headerRowDxfId="8">
+  <autoFilter ref="A1:G40" xr:uid="{74C06549-5BDA-49EA-8217-9DE86359CCAF}"/>
+  <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{94AE38D3-5B70-43B1-956A-6DFBCCC3FA71}" name="Feature"/>
     <tableColumn id="9" xr3:uid="{39B338AE-1DE7-47E0-9DFF-EB558B693D9E}" name="Sub Feature"/>
     <tableColumn id="11" xr3:uid="{8F685D88-2001-49B6-A560-44AC61A85751}" name="Document"/>
-    <tableColumn id="10" xr3:uid="{4B57D4E1-7F53-4AB1-93B7-628D0D759AD9}" name="UI" dataDxfId="4"/>
-    <tableColumn id="13" xr3:uid="{3B45BC65-AA1D-4611-BFDF-489E623921CC}" name="Positive-negative" dataDxfId="3"/>
-    <tableColumn id="2" xr3:uid="{2B877830-769C-4915-8F5E-FA01A5B40D0A}" name="Scenario" dataDxfId="2"/>
+    <tableColumn id="10" xr3:uid="{4B57D4E1-7F53-4AB1-93B7-628D0D759AD9}" name="UI" dataDxfId="7"/>
+    <tableColumn id="13" xr3:uid="{3B45BC65-AA1D-4611-BFDF-489E623921CC}" name="Positive-negative" dataDxfId="6"/>
+    <tableColumn id="2" xr3:uid="{2B877830-769C-4915-8F5E-FA01A5B40D0A}" name="Scenario" dataDxfId="1"/>
+    <tableColumn id="3" xr3:uid="{5F61A9FF-ECAD-4E09-97CB-6378A95FA907}" name="Scenario #" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -633,10 +676,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B26A05CD-DD6F-435A-8EFB-058B6AB8AAF4}">
-  <dimension ref="A1:F40"/>
+  <dimension ref="A1:G40"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F53" sqref="F53"/>
+      <selection activeCell="G44" sqref="G44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -647,9 +690,10 @@
     <col min="4" max="4" width="5.85546875" style="6" customWidth="1"/>
     <col min="5" max="5" width="9.7109375" style="6" customWidth="1"/>
     <col min="6" max="6" width="113.28515625" style="7" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.140625" style="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -668,8 +712,11 @@
       <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G1" s="12" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>5</v>
       </c>
@@ -680,8 +727,9 @@
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
       <c r="F2" s="5"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G2" s="14"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
         <v>5</v>
       </c>
@@ -694,8 +742,11 @@
       <c r="F3" s="10" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G3" s="13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
         <v>5</v>
       </c>
@@ -710,8 +761,11 @@
       <c r="F4" s="10" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G4" s="13">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
         <v>5</v>
       </c>
@@ -726,8 +780,11 @@
       <c r="F5" s="10" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G5" s="13">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>5</v>
       </c>
@@ -738,8 +795,9 @@
       <c r="D6" s="4"/>
       <c r="E6" s="4"/>
       <c r="F6" s="5"/>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G6" s="14"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
         <v>5</v>
       </c>
@@ -752,8 +810,11 @@
       <c r="F7" s="10" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G7" s="13">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="8" t="s">
         <v>5</v>
       </c>
@@ -768,8 +829,11 @@
       <c r="F8" s="10" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G8" s="13">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
         <v>5</v>
       </c>
@@ -786,8 +850,11 @@
       <c r="F9" s="10" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G9" s="13">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="8" t="s">
         <v>5</v>
       </c>
@@ -804,8 +871,11 @@
       <c r="F10" s="10" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G10" s="13">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
         <v>5</v>
       </c>
@@ -822,8 +892,11 @@
       <c r="F11" s="10" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G11" s="13">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="8" t="s">
         <v>5</v>
       </c>
@@ -840,8 +913,11 @@
       <c r="F12" s="10" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G12" s="13">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
         <v>5</v>
       </c>
@@ -858,8 +934,11 @@
       <c r="F13" s="10" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G13" s="13">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="8" t="s">
         <v>5</v>
       </c>
@@ -876,8 +955,11 @@
       <c r="F14" s="10" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G14" s="13">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>5</v>
       </c>
@@ -888,8 +970,9 @@
       <c r="D15" s="4"/>
       <c r="E15" s="4"/>
       <c r="F15" s="5"/>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G15" s="14"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="8" t="s">
         <v>5</v>
       </c>
@@ -902,8 +985,11 @@
       <c r="F16" s="10" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G16" s="13">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="8" t="s">
         <v>5</v>
       </c>
@@ -918,8 +1004,11 @@
       <c r="F17" s="10" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G17" s="13">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="8" t="s">
         <v>5</v>
       </c>
@@ -934,8 +1023,11 @@
       <c r="F18" s="10" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G18" s="13">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>30</v>
       </c>
@@ -946,8 +1038,9 @@
       <c r="D19" s="4"/>
       <c r="E19" s="4"/>
       <c r="F19" s="5"/>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G19" s="14"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="8" t="s">
         <v>30</v>
       </c>
@@ -960,8 +1053,11 @@
       <c r="F20" s="10" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G20" s="13">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="8" t="s">
         <v>30</v>
       </c>
@@ -976,8 +1072,11 @@
       <c r="F21" s="10" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G21" s="13">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="8" t="s">
         <v>30</v>
       </c>
@@ -992,8 +1091,11 @@
       <c r="F22" s="10" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G22" s="13">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>30</v>
       </c>
@@ -1004,8 +1106,9 @@
       <c r="D23" s="4"/>
       <c r="E23" s="4"/>
       <c r="F23" s="5"/>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G23" s="14"/>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="8" t="s">
         <v>30</v>
       </c>
@@ -1020,8 +1123,11 @@
       <c r="F24" s="10" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G24" s="13">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="8" t="s">
         <v>30</v>
       </c>
@@ -1036,8 +1142,11 @@
       <c r="F25" s="10" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G25" s="13">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="8" t="s">
         <v>30</v>
       </c>
@@ -1052,8 +1161,11 @@
       <c r="F26" s="10" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G26" s="13">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="8" t="s">
         <v>30</v>
       </c>
@@ -1070,8 +1182,11 @@
       <c r="F27" s="10" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="28" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G27" s="13">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
         <v>30</v>
       </c>
@@ -1082,8 +1197,9 @@
       <c r="D28" s="4"/>
       <c r="E28" s="4"/>
       <c r="F28" s="5"/>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G28" s="14"/>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="8" t="s">
         <v>30</v>
       </c>
@@ -1098,8 +1214,11 @@
       <c r="F29" s="8" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G29" s="13">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="8" t="s">
         <v>30</v>
       </c>
@@ -1114,8 +1233,11 @@
       <c r="F30" s="10" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G30" s="13">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="8" t="s">
         <v>30</v>
       </c>
@@ -1130,8 +1252,11 @@
       <c r="F31" s="10" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G31" s="13">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="8" t="s">
         <v>30</v>
       </c>
@@ -1146,8 +1271,11 @@
       <c r="F32" s="10" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G32" s="13">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="8" t="s">
         <v>30</v>
       </c>
@@ -1162,8 +1290,11 @@
       <c r="F33" s="10" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G33" s="13">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
         <v>30</v>
       </c>
@@ -1174,8 +1305,9 @@
       <c r="D34" s="4"/>
       <c r="E34" s="4"/>
       <c r="F34" s="5"/>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G34" s="14"/>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="8" t="s">
         <v>30</v>
       </c>
@@ -1190,8 +1322,11 @@
       <c r="F35" s="10" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G35" s="13">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="8" t="s">
         <v>30</v>
       </c>
@@ -1208,8 +1343,11 @@
       <c r="F36" s="10" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G36" s="13">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="8" t="s">
         <v>30</v>
       </c>
@@ -1224,8 +1362,11 @@
       <c r="F37" s="10" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G37" s="13">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="8" t="s">
         <v>30</v>
       </c>
@@ -1242,8 +1383,11 @@
       <c r="F38" s="10" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G38" s="13">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
         <v>30</v>
       </c>
@@ -1254,8 +1398,9 @@
       <c r="D39" s="4"/>
       <c r="E39" s="4"/>
       <c r="F39" s="5"/>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G39" s="14"/>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="8" t="s">
         <v>30</v>
       </c>
@@ -1268,16 +1413,31 @@
       <c r="F40" s="10" t="s">
         <v>52</v>
       </c>
+      <c r="G40" s="13">
+        <v>29</v>
+      </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="D1:D1048576">
-    <cfRule type="cellIs" dxfId="1" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="8" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E1:E1048576">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
       <formula>"X"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G1:G1048576">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>